<commit_message>
npb plot with error bar
</commit_message>
<xml_diff>
--- a/benchmark/NPB3.0-omp-C.xlsx
+++ b/benchmark/NPB3.0-omp-C.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ninek\Desktop\sable-wasm\benchmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/67c04eb2ba898580/Desktop/sable-wasm/benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4153BB00-8B7F-4DB2-BF16-36CF2544A4D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="13_ncr:1_{4153BB00-8B7F-4DB2-BF16-36CF2544A4D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E03FB09B-EF9D-4115-B3F7-A69033352C5A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,11 @@
     <sheet name="2" sheetId="3" r:id="rId3"/>
     <sheet name="3" sheetId="4" r:id="rId4"/>
     <sheet name="4" sheetId="5" r:id="rId5"/>
+    <sheet name="5" sheetId="6" r:id="rId6"/>
+    <sheet name="6" sheetId="7" r:id="rId7"/>
+    <sheet name="7" sheetId="8" r:id="rId8"/>
+    <sheet name="8" sheetId="9" r:id="rId9"/>
+    <sheet name="9" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -92,30 +97,6 @@
   </si>
   <si>
     <t>SP</t>
-  </si>
-  <si>
-    <t>BT.A</t>
-  </si>
-  <si>
-    <t>CG.A</t>
-  </si>
-  <si>
-    <t>EP.A</t>
-  </si>
-  <si>
-    <t>FT.A</t>
-  </si>
-  <si>
-    <t>IS.A</t>
-  </si>
-  <si>
-    <t>LU.W</t>
-  </si>
-  <si>
-    <t>MG.A</t>
-  </si>
-  <si>
-    <t>SP.A</t>
   </si>
 </sst>
 </file>
@@ -188,6 +169,28 @@
     <tableColumn id="11" xr3:uid="{284CA680-0B10-41EE-88B8-24B5FA29A3BC}" name="Wasmer-LLVM(Naive)"/>
     <tableColumn id="12" xr3:uid="{83C310D8-81FF-4508-8A93-0A10F83C6A76}" name="Wasmer-LLVM(Opt)"/>
     <tableColumn id="13" xr3:uid="{9A4859E5-D815-4394-B2FB-34D16BE5CAA8}" name="Wasmer-LLVM(SIMD)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4AC1CD61-37BF-43F0-B88E-68506F7EA2CF}" name="Table35637891011" displayName="Table35637891011" ref="A1:M9" totalsRowShown="0">
+  <autoFilter ref="A1:M9" xr:uid="{863CB8EB-527D-46D9-B248-5577496A7E63}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{25641D9D-6FF4-4ACE-990A-92C57A510EE0}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{FA550A18-22ED-4A82-A9AE-962D0CA188F9}" name="SableWasm(Naive)"/>
+    <tableColumn id="3" xr3:uid="{4FD02F89-98C0-41C1-A8C0-59D964BC9947}" name="SableWasm(Opt)"/>
+    <tableColumn id="4" xr3:uid="{FABDAFAE-2CC8-4EE6-9E08-4505201CA8FB}" name="SableWasm(SIMD)"/>
+    <tableColumn id="5" xr3:uid="{21272102-2A4B-425D-9110-DE019A034D6D}" name="Wasmtime(Naive)"/>
+    <tableColumn id="6" xr3:uid="{8DBEB767-A2F8-4AA7-B742-95D684F6C302}" name="Wasmtime(Opt)"/>
+    <tableColumn id="7" xr3:uid="{DF380F3B-433C-418C-A598-B43A3B756088}" name="Wasmtime(SIMD)"/>
+    <tableColumn id="8" xr3:uid="{0B29D6DC-CB12-43A8-A249-B1BF8AF03496}" name="Wasmer-Cranelift(Naive)"/>
+    <tableColumn id="9" xr3:uid="{DBE65E4E-8A98-4D1D-85D5-B1D76C05C50B}" name="Wasmer-Cranelift(Opt)"/>
+    <tableColumn id="10" xr3:uid="{5641A135-280B-4FC6-A337-AD37B0F4E08F}" name="Wasmer-Cranelift(SIMD)"/>
+    <tableColumn id="11" xr3:uid="{BD5EEC1F-88BC-4AB4-9717-E2CD65F1765A}" name="Wasmer-LLVM(Naive)"/>
+    <tableColumn id="12" xr3:uid="{E1CE1422-3DA8-4886-BA3B-5148784A89D2}" name="Wasmer-LLVM(Opt)"/>
+    <tableColumn id="13" xr3:uid="{BCBD2A7D-B8AF-4444-836C-6D862726E25A}" name="Wasmer-LLVM(SIMD)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -276,6 +279,94 @@
     <tableColumn id="11" xr3:uid="{E10A4980-FF35-4E37-9C87-ABE178039462}" name="Wasmer-LLVM(Naive)"/>
     <tableColumn id="12" xr3:uid="{F587D74F-4B99-4F6E-8275-E14CD35F576F}" name="Wasmer-LLVM(Opt)"/>
     <tableColumn id="13" xr3:uid="{64FBB0CC-D1EA-4D4F-9968-FAD21A0C9484}" name="Wasmer-LLVM(SIMD)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{45B929F5-BBDD-434B-9439-8C746F51001E}" name="Table35637" displayName="Table35637" ref="A1:M9" totalsRowShown="0">
+  <autoFilter ref="A1:M9" xr:uid="{863CB8EB-527D-46D9-B248-5577496A7E63}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{90C9EEBA-3D5B-4BDB-B102-26B5043807A8}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{45661EF0-6C21-461F-9AE7-6C5208963371}" name="SableWasm(Naive)"/>
+    <tableColumn id="3" xr3:uid="{753DE7DC-61AA-47CE-909B-CC77A0B7311B}" name="SableWasm(Opt)"/>
+    <tableColumn id="4" xr3:uid="{589D7AC8-2FFD-46EF-8380-66BB7168359E}" name="SableWasm(SIMD)"/>
+    <tableColumn id="5" xr3:uid="{8EB7374F-E60A-474B-B97F-F78CE2CBD5B4}" name="Wasmtime(Naive)"/>
+    <tableColumn id="6" xr3:uid="{C28CD88D-91B6-49FE-AF81-3564D0777C7C}" name="Wasmtime(Opt)"/>
+    <tableColumn id="7" xr3:uid="{F2473EFC-5E2B-4378-90C0-B5EC22DBADC4}" name="Wasmtime(SIMD)"/>
+    <tableColumn id="8" xr3:uid="{40A4DD4A-6A99-41E2-8322-BF848A3D53A1}" name="Wasmer-Cranelift(Naive)"/>
+    <tableColumn id="9" xr3:uid="{E17A8085-CEAC-4D12-A092-F0F583BD870B}" name="Wasmer-Cranelift(Opt)"/>
+    <tableColumn id="10" xr3:uid="{A53F236F-EB08-4D12-82C6-A9A25A0DAC82}" name="Wasmer-Cranelift(SIMD)"/>
+    <tableColumn id="11" xr3:uid="{9E5452A8-24BD-43C2-B725-8E7F9E37688C}" name="Wasmer-LLVM(Naive)"/>
+    <tableColumn id="12" xr3:uid="{462152F5-DE27-4B64-8FC3-52FE23076513}" name="Wasmer-LLVM(Opt)"/>
+    <tableColumn id="13" xr3:uid="{BC77B6F4-9D02-45BC-AE82-9E10211DF148}" name="Wasmer-LLVM(SIMD)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F4619F90-C345-42B6-8992-2D7DB40D96EF}" name="Table356378" displayName="Table356378" ref="A1:M9" totalsRowShown="0">
+  <autoFilter ref="A1:M9" xr:uid="{863CB8EB-527D-46D9-B248-5577496A7E63}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{D40EB63A-3992-4B2F-9A11-1B7D51429665}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{0186C410-7CC1-41D3-9395-ABFDA4E67EBC}" name="SableWasm(Naive)"/>
+    <tableColumn id="3" xr3:uid="{1FB11484-F1B6-46B4-9A15-1ADCEE1B6D0B}" name="SableWasm(Opt)"/>
+    <tableColumn id="4" xr3:uid="{FF9E40DF-8736-49E5-AA37-05D28494FC3D}" name="SableWasm(SIMD)"/>
+    <tableColumn id="5" xr3:uid="{019E8FA1-BAFF-4EFA-A525-3416A47B8C7E}" name="Wasmtime(Naive)"/>
+    <tableColumn id="6" xr3:uid="{7309011D-9812-483E-AB76-2DD703351743}" name="Wasmtime(Opt)"/>
+    <tableColumn id="7" xr3:uid="{7F3ECDAF-16ED-48BE-A12C-A277B990FD11}" name="Wasmtime(SIMD)"/>
+    <tableColumn id="8" xr3:uid="{3985E169-D13C-4A91-858C-9CE8C6E6EC2D}" name="Wasmer-Cranelift(Naive)"/>
+    <tableColumn id="9" xr3:uid="{D98CD195-C10C-4226-A9DF-024B456023D4}" name="Wasmer-Cranelift(Opt)"/>
+    <tableColumn id="10" xr3:uid="{F387ACF9-1810-406A-AA3C-9F1DDDDE64B9}" name="Wasmer-Cranelift(SIMD)"/>
+    <tableColumn id="11" xr3:uid="{7A59EAEC-A656-48A7-952A-7D681F0DBCFA}" name="Wasmer-LLVM(Naive)"/>
+    <tableColumn id="12" xr3:uid="{330B77AB-49C6-4891-B61B-E5F815A23629}" name="Wasmer-LLVM(Opt)"/>
+    <tableColumn id="13" xr3:uid="{51126657-5080-467F-AEAF-E2F7229C1950}" name="Wasmer-LLVM(SIMD)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5CDE90B8-6778-4322-A014-37F9A97D0D33}" name="Table3563789" displayName="Table3563789" ref="A1:M9" totalsRowShown="0">
+  <autoFilter ref="A1:M9" xr:uid="{863CB8EB-527D-46D9-B248-5577496A7E63}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{CF91F862-FF61-4137-BBF0-972E794DB4DF}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{8A97A4D9-CD92-4264-9FD6-1BE7E7B216E4}" name="SableWasm(Naive)"/>
+    <tableColumn id="3" xr3:uid="{F3522C36-0E17-4F46-B7E7-9D3980CC11A6}" name="SableWasm(Opt)"/>
+    <tableColumn id="4" xr3:uid="{D283F8BC-758C-496B-9508-3559A3889EA1}" name="SableWasm(SIMD)"/>
+    <tableColumn id="5" xr3:uid="{BC006ED7-1B6E-4C65-A903-012A3FE1E2B5}" name="Wasmtime(Naive)"/>
+    <tableColumn id="6" xr3:uid="{40A22732-FF63-47D1-B534-BCFB2EAE9986}" name="Wasmtime(Opt)"/>
+    <tableColumn id="7" xr3:uid="{42E3B379-E083-4CA8-8411-F75B512B1873}" name="Wasmtime(SIMD)"/>
+    <tableColumn id="8" xr3:uid="{C696E715-473F-4C41-8C12-96BB018DAFD4}" name="Wasmer-Cranelift(Naive)"/>
+    <tableColumn id="9" xr3:uid="{D98DFCEA-C208-496B-811A-50AC32EB0AEE}" name="Wasmer-Cranelift(Opt)"/>
+    <tableColumn id="10" xr3:uid="{463928E8-7D79-45D2-ABC3-9105DFD37C17}" name="Wasmer-Cranelift(SIMD)"/>
+    <tableColumn id="11" xr3:uid="{606BEA7D-51D2-4CB3-841D-E0134A437E62}" name="Wasmer-LLVM(Naive)"/>
+    <tableColumn id="12" xr3:uid="{AE2D0124-2D93-4376-A535-E5A0C1D87E67}" name="Wasmer-LLVM(Opt)"/>
+    <tableColumn id="13" xr3:uid="{508FC410-82C8-4AEC-9F50-F565A70EE967}" name="Wasmer-LLVM(SIMD)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{C5D2C8E1-64B2-4C3B-93BF-E68183752C5E}" name="Table356378910" displayName="Table356378910" ref="A1:M9" totalsRowShown="0">
+  <autoFilter ref="A1:M9" xr:uid="{863CB8EB-527D-46D9-B248-5577496A7E63}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{4A3CA1BD-AD02-4BDF-A021-24DB02D690DD}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{6BD2081B-0DE3-4A97-ABEE-3CD68AE299CF}" name="SableWasm(Naive)"/>
+    <tableColumn id="3" xr3:uid="{CB3C7FF9-C43A-4D9F-A3DB-B3A36E5233BB}" name="SableWasm(Opt)"/>
+    <tableColumn id="4" xr3:uid="{1558DC81-B5FD-4B48-8121-185944A20313}" name="SableWasm(SIMD)"/>
+    <tableColumn id="5" xr3:uid="{F754AA8E-AA9C-4089-9973-2A6761D82F7C}" name="Wasmtime(Naive)"/>
+    <tableColumn id="6" xr3:uid="{A8A203C5-DEE7-42EF-A440-53DBCA518A47}" name="Wasmtime(Opt)"/>
+    <tableColumn id="7" xr3:uid="{64FC7C68-0570-4976-8841-24EE25C982E3}" name="Wasmtime(SIMD)"/>
+    <tableColumn id="8" xr3:uid="{A136040B-6980-4285-B71C-EE58A6BAFA97}" name="Wasmer-Cranelift(Naive)"/>
+    <tableColumn id="9" xr3:uid="{5B73568C-1559-46F6-B296-16F58868B301}" name="Wasmer-Cranelift(Opt)"/>
+    <tableColumn id="10" xr3:uid="{D78F4272-2FC8-44A2-A50A-20561D5BE294}" name="Wasmer-Cranelift(SIMD)"/>
+    <tableColumn id="11" xr3:uid="{56E515B9-466C-43AD-B098-D5E1CAAFAE78}" name="Wasmer-LLVM(Naive)"/>
+    <tableColumn id="12" xr3:uid="{4F0DB87B-41C1-413A-8061-5F57E83C6FB9}" name="Wasmer-LLVM(Opt)"/>
+    <tableColumn id="13" xr3:uid="{7D0A523A-B54A-4D94-8369-246C7D227900}" name="Wasmer-LLVM(SIMD)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -547,7 +638,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,23 +885,23 @@
       <c r="G6" t="e">
         <v>#N/A</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>0.37</v>
-      </c>
-      <c r="J6">
-        <v>0.38</v>
-      </c>
-      <c r="K6">
-        <v>0.31</v>
-      </c>
-      <c r="L6">
-        <v>0.21</v>
-      </c>
-      <c r="M6">
-        <v>0.2</v>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -944,12 +1035,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA394A1-FBB6-4117-9EB6-B156D9397E4A}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,40 +1106,40 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>104.37</v>
+        <v>102.68</v>
       </c>
       <c r="C2">
-        <v>56.49</v>
+        <v>56.53</v>
       </c>
       <c r="D2">
-        <v>50.78</v>
+        <v>49.78</v>
       </c>
       <c r="E2">
-        <v>124.86</v>
+        <v>124.19</v>
       </c>
       <c r="F2">
-        <v>51.74</v>
+        <v>51.67</v>
       </c>
       <c r="G2">
-        <v>47.63</v>
+        <v>47.61</v>
       </c>
       <c r="H2">
-        <v>307.87</v>
+        <v>303.27</v>
       </c>
       <c r="I2">
-        <v>108.05</v>
+        <v>107.79</v>
       </c>
       <c r="J2">
-        <v>89.18</v>
+        <v>88.6</v>
       </c>
       <c r="K2">
-        <v>182.98</v>
+        <v>182.65</v>
       </c>
       <c r="L2">
-        <v>65.98</v>
+        <v>66.150000000000006</v>
       </c>
       <c r="M2">
-        <v>58.07</v>
+        <v>58.09</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1056,7 +1147,7 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>2.4700000000000002</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="C3">
         <v>0.76</v>
@@ -1065,31 +1156,31 @@
         <v>0.77</v>
       </c>
       <c r="E3">
-        <v>2.41</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="F3">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="H3">
-        <v>5.73</v>
+        <v>5.2</v>
       </c>
       <c r="I3">
-        <v>2.04</v>
+        <v>1.89</v>
       </c>
       <c r="J3">
-        <v>2.11</v>
+        <v>1.91</v>
       </c>
       <c r="K3">
-        <v>3.03</v>
+        <v>2.87</v>
       </c>
       <c r="L3">
-        <v>1.78</v>
+        <v>1.84</v>
       </c>
       <c r="M3">
-        <v>1.78</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1097,40 +1188,40 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>20.79</v>
+        <v>20.86</v>
       </c>
       <c r="C4">
-        <v>13.87</v>
+        <v>13.89</v>
       </c>
       <c r="D4">
-        <v>13.66</v>
+        <v>13.86</v>
       </c>
       <c r="E4">
-        <v>23.53</v>
+        <v>24.29</v>
       </c>
       <c r="F4">
-        <v>17.52</v>
+        <v>17.66</v>
       </c>
       <c r="G4">
-        <v>17.170000000000002</v>
+        <v>17.28</v>
       </c>
       <c r="H4">
-        <v>27.55</v>
+        <v>27.51</v>
       </c>
       <c r="I4">
-        <v>18.93</v>
+        <v>19.059999999999999</v>
       </c>
       <c r="J4">
-        <v>18.760000000000002</v>
+        <v>18.72</v>
       </c>
       <c r="K4">
-        <v>38.450000000000003</v>
+        <v>38.31</v>
       </c>
       <c r="L4">
-        <v>19.57</v>
+        <v>19.64</v>
       </c>
       <c r="M4">
-        <v>19.04</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1138,7 +1229,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>9.7200000000000006</v>
+        <v>9.66</v>
       </c>
       <c r="C5" t="e">
         <v>#N/A</v>
@@ -1147,7 +1238,7 @@
         <v>#N/A</v>
       </c>
       <c r="E5">
-        <v>7.69</v>
+        <v>7.63</v>
       </c>
       <c r="F5" t="e">
         <v>#N/A</v>
@@ -1156,7 +1247,7 @@
         <v>#N/A</v>
       </c>
       <c r="H5">
-        <v>21.34</v>
+        <v>21.62</v>
       </c>
       <c r="I5" t="e">
         <v>#N/A</v>
@@ -1165,7 +1256,7 @@
         <v>#N/A</v>
       </c>
       <c r="K5">
-        <v>10.89</v>
+        <v>11.32</v>
       </c>
       <c r="L5" t="e">
         <v>#N/A</v>
@@ -1196,23 +1287,23 @@
       <c r="G6" t="e">
         <v>#N/A</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>0.37</v>
-      </c>
-      <c r="J6">
-        <v>0.36</v>
-      </c>
-      <c r="K6">
-        <v>0.31</v>
-      </c>
-      <c r="L6">
-        <v>0.21</v>
-      </c>
-      <c r="M6">
-        <v>0.21</v>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1220,40 +1311,40 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>8.94</v>
+        <v>8.8699999999999992</v>
       </c>
       <c r="C7">
-        <v>3.29</v>
+        <v>3.31</v>
       </c>
       <c r="D7">
-        <v>3.23</v>
+        <v>3.13</v>
       </c>
       <c r="E7">
-        <v>13.97</v>
+        <v>14.1</v>
       </c>
       <c r="F7">
         <v>4.12</v>
       </c>
       <c r="G7">
-        <v>3.95</v>
+        <v>3.85</v>
       </c>
       <c r="H7">
-        <v>31.9</v>
+        <v>33.29</v>
       </c>
       <c r="I7">
-        <v>6.24</v>
+        <v>6.32</v>
       </c>
       <c r="J7">
         <v>5.78</v>
       </c>
       <c r="K7">
-        <v>21.95</v>
+        <v>22</v>
       </c>
       <c r="L7">
-        <v>5.62</v>
+        <v>5.49</v>
       </c>
       <c r="M7">
-        <v>5.23</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1261,40 +1352,40 @@
         <v>19</v>
       </c>
       <c r="B8">
-        <v>3.12</v>
+        <v>3.2</v>
       </c>
       <c r="C8">
-        <v>1.25</v>
+        <v>1.26</v>
       </c>
       <c r="D8">
-        <v>1.24</v>
+        <v>1.23</v>
       </c>
       <c r="E8">
-        <v>4.24</v>
+        <v>4.33</v>
       </c>
       <c r="F8">
-        <v>1.32</v>
+        <v>1.57</v>
       </c>
       <c r="G8">
-        <v>1.36</v>
+        <v>1.37</v>
       </c>
       <c r="H8">
-        <v>17.899999999999999</v>
+        <v>17.78</v>
       </c>
       <c r="I8">
-        <v>2.76</v>
+        <v>2.74</v>
       </c>
       <c r="J8">
-        <v>2.72</v>
+        <v>2.7</v>
       </c>
       <c r="K8">
-        <v>6.2</v>
+        <v>6.19</v>
       </c>
       <c r="L8">
-        <v>1.36</v>
+        <v>1.35</v>
       </c>
       <c r="M8">
-        <v>1.37</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1302,40 +1393,40 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>59.4</v>
+        <v>59.1</v>
       </c>
       <c r="C9">
-        <v>24.61</v>
+        <v>24.57</v>
       </c>
       <c r="D9">
-        <v>22.7</v>
+        <v>22.75</v>
       </c>
       <c r="E9">
-        <v>93.78</v>
+        <v>94.68</v>
       </c>
       <c r="F9">
-        <v>28.11</v>
+        <v>27.78</v>
       </c>
       <c r="G9" t="e">
         <v>#N/A</v>
       </c>
       <c r="H9">
-        <v>340.82</v>
+        <v>343.12</v>
       </c>
       <c r="I9">
-        <v>45.45</v>
+        <v>45.46</v>
       </c>
       <c r="J9">
-        <v>36.17</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="K9">
-        <v>143.56</v>
+        <v>145.84</v>
       </c>
       <c r="L9">
-        <v>33.51</v>
+        <v>33.46</v>
       </c>
       <c r="M9">
-        <v>81.150000000000006</v>
+        <v>80.819999999999993</v>
       </c>
     </row>
   </sheetData>
@@ -1346,12 +1437,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6EBF94-02A4-4DB1-BF3D-E80F1705BA4C}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,40 +1508,40 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>102.36</v>
+        <v>104.37</v>
       </c>
       <c r="C2">
-        <v>56.5</v>
+        <v>56.49</v>
       </c>
       <c r="D2">
-        <v>50.37</v>
+        <v>50.78</v>
       </c>
       <c r="E2">
-        <v>124.59</v>
+        <v>124.86</v>
       </c>
       <c r="F2">
-        <v>51.88</v>
+        <v>51.74</v>
       </c>
       <c r="G2">
-        <v>47.59</v>
+        <v>47.63</v>
       </c>
       <c r="H2">
-        <v>303.47000000000003</v>
+        <v>307.87</v>
       </c>
       <c r="I2">
-        <v>107.24</v>
+        <v>108.05</v>
       </c>
       <c r="J2">
-        <v>88.41</v>
+        <v>89.18</v>
       </c>
       <c r="K2">
-        <v>181.2</v>
+        <v>182.98</v>
       </c>
       <c r="L2">
-        <v>66.400000000000006</v>
+        <v>65.98</v>
       </c>
       <c r="M2">
-        <v>57.86</v>
+        <v>58.07</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1458,40 +1549,40 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>2.23</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="C3">
-        <v>0.8</v>
+        <v>0.76</v>
       </c>
       <c r="D3">
         <v>0.77</v>
       </c>
       <c r="E3">
-        <v>2.13</v>
+        <v>2.41</v>
       </c>
       <c r="F3">
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
       <c r="G3">
-        <v>0.91</v>
+        <v>0.9</v>
       </c>
       <c r="H3">
-        <v>5.44</v>
+        <v>5.73</v>
       </c>
       <c r="I3">
-        <v>1.96</v>
+        <v>2.04</v>
       </c>
       <c r="J3">
-        <v>1.92</v>
+        <v>2.11</v>
       </c>
       <c r="K3">
-        <v>2.87</v>
+        <v>3.03</v>
       </c>
       <c r="L3">
-        <v>1.79</v>
+        <v>1.78</v>
       </c>
       <c r="M3">
-        <v>1.75</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1499,40 +1590,40 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>20.81</v>
+        <v>20.79</v>
       </c>
       <c r="C4">
         <v>13.87</v>
       </c>
       <c r="D4">
-        <v>13.87</v>
+        <v>13.66</v>
       </c>
       <c r="E4">
-        <v>23.64</v>
+        <v>23.53</v>
       </c>
       <c r="F4">
-        <v>17.63</v>
+        <v>17.52</v>
       </c>
       <c r="G4">
-        <v>17.149999999999999</v>
+        <v>17.170000000000002</v>
       </c>
       <c r="H4">
-        <v>27.56</v>
+        <v>27.55</v>
       </c>
       <c r="I4">
-        <v>19</v>
+        <v>18.93</v>
       </c>
       <c r="J4">
         <v>18.760000000000002</v>
       </c>
       <c r="K4">
-        <v>38.51</v>
+        <v>38.450000000000003</v>
       </c>
       <c r="L4">
-        <v>19.559999999999999</v>
+        <v>19.57</v>
       </c>
       <c r="M4">
-        <v>18.989999999999998</v>
+        <v>19.04</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1540,7 +1631,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>9.6300000000000008</v>
+        <v>9.7200000000000006</v>
       </c>
       <c r="C5" t="e">
         <v>#N/A</v>
@@ -1549,7 +1640,7 @@
         <v>#N/A</v>
       </c>
       <c r="E5">
-        <v>7.6</v>
+        <v>7.69</v>
       </c>
       <c r="F5" t="e">
         <v>#N/A</v>
@@ -1558,7 +1649,7 @@
         <v>#N/A</v>
       </c>
       <c r="H5">
-        <v>21.29</v>
+        <v>21.34</v>
       </c>
       <c r="I5" t="e">
         <v>#N/A</v>
@@ -1567,7 +1658,7 @@
         <v>#N/A</v>
       </c>
       <c r="K5">
-        <v>10.75</v>
+        <v>10.89</v>
       </c>
       <c r="L5" t="e">
         <v>#N/A</v>
@@ -1598,23 +1689,23 @@
       <c r="G6" t="e">
         <v>#N/A</v>
       </c>
-      <c r="H6">
-        <v>1.01</v>
-      </c>
-      <c r="I6">
-        <v>0.38</v>
-      </c>
-      <c r="J6">
-        <v>0.37</v>
-      </c>
-      <c r="K6">
-        <v>0.31</v>
-      </c>
-      <c r="L6">
-        <v>0.21</v>
-      </c>
-      <c r="M6">
-        <v>0.21</v>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1622,37 +1713,37 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>9.1199999999999992</v>
+        <v>8.94</v>
       </c>
       <c r="C7">
-        <v>3.39</v>
+        <v>3.29</v>
       </c>
       <c r="D7">
-        <v>3.68</v>
+        <v>3.23</v>
       </c>
       <c r="E7">
-        <v>13.92</v>
+        <v>13.97</v>
       </c>
       <c r="F7">
-        <v>4.0599999999999996</v>
+        <v>4.12</v>
       </c>
       <c r="G7">
-        <v>3.91</v>
+        <v>3.95</v>
       </c>
       <c r="H7">
-        <v>32.04</v>
+        <v>31.9</v>
       </c>
       <c r="I7">
-        <v>6.28</v>
+        <v>6.24</v>
       </c>
       <c r="J7">
-        <v>5.73</v>
+        <v>5.78</v>
       </c>
       <c r="K7">
-        <v>22</v>
+        <v>21.95</v>
       </c>
       <c r="L7">
-        <v>5.55</v>
+        <v>5.62</v>
       </c>
       <c r="M7">
         <v>5.23</v>
@@ -1666,37 +1757,37 @@
         <v>3.12</v>
       </c>
       <c r="C8">
-        <v>1.24</v>
+        <v>1.25</v>
       </c>
       <c r="D8">
         <v>1.24</v>
       </c>
       <c r="E8">
-        <v>4.3099999999999996</v>
+        <v>4.24</v>
       </c>
       <c r="F8">
-        <v>1.34</v>
+        <v>1.32</v>
       </c>
       <c r="G8">
-        <v>1.38</v>
+        <v>1.36</v>
       </c>
       <c r="H8">
-        <v>18.62</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="I8">
         <v>2.76</v>
       </c>
       <c r="J8">
-        <v>2.73</v>
+        <v>2.72</v>
       </c>
       <c r="K8">
         <v>6.2</v>
       </c>
       <c r="L8">
-        <v>1.38</v>
+        <v>1.36</v>
       </c>
       <c r="M8">
-        <v>1.36</v>
+        <v>1.37</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1704,40 +1795,40 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>59.06</v>
+        <v>59.4</v>
       </c>
       <c r="C9">
-        <v>24.63</v>
+        <v>24.61</v>
       </c>
       <c r="D9">
-        <v>22.74</v>
+        <v>22.7</v>
       </c>
       <c r="E9">
-        <v>95.33</v>
+        <v>93.78</v>
       </c>
       <c r="F9">
-        <v>27.59</v>
+        <v>28.11</v>
       </c>
       <c r="G9" t="e">
         <v>#N/A</v>
       </c>
       <c r="H9">
-        <v>340.57</v>
+        <v>340.82</v>
       </c>
       <c r="I9">
-        <v>45.56</v>
+        <v>45.45</v>
       </c>
       <c r="J9">
-        <v>35.840000000000003</v>
+        <v>36.17</v>
       </c>
       <c r="K9">
-        <v>145.88</v>
+        <v>143.56</v>
       </c>
       <c r="L9">
-        <v>33.380000000000003</v>
+        <v>33.51</v>
       </c>
       <c r="M9">
-        <v>81.099999999999994</v>
+        <v>81.150000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -1748,12 +1839,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E4BC65-974B-4C0A-9F10-9CAD64070E0C}">
-  <dimension ref="A1:M21"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6EBF94-02A4-4DB1-BF3D-E80F1705BA4C}">
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1819,31 +1910,40 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>103.57</v>
+        <v>102.36</v>
       </c>
       <c r="C2">
-        <v>56.25</v>
+        <v>56.5</v>
       </c>
       <c r="D2">
-        <v>50.7</v>
+        <v>50.37</v>
       </c>
       <c r="E2">
-        <v>125.33</v>
+        <v>124.59</v>
       </c>
       <c r="F2">
-        <v>51.5</v>
+        <v>51.88</v>
       </c>
       <c r="G2">
-        <v>47.56</v>
+        <v>47.59</v>
       </c>
       <c r="H2">
-        <v>304.19</v>
+        <v>303.47000000000003</v>
       </c>
       <c r="I2">
-        <v>107.32</v>
+        <v>107.24</v>
       </c>
       <c r="J2">
-        <v>88.19</v>
+        <v>88.41</v>
+      </c>
+      <c r="K2">
+        <v>181.2</v>
+      </c>
+      <c r="L2">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="M2">
+        <v>57.86</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1851,31 +1951,40 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>2.29</v>
+        <v>2.23</v>
       </c>
       <c r="C3">
+        <v>0.8</v>
+      </c>
+      <c r="D3">
         <v>0.77</v>
       </c>
-      <c r="D3">
-        <v>0.75</v>
-      </c>
       <c r="E3">
-        <v>2.14</v>
+        <v>2.13</v>
       </c>
       <c r="F3">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="G3">
-        <v>0.96</v>
+        <v>0.91</v>
       </c>
       <c r="H3">
-        <v>5.4</v>
+        <v>5.44</v>
       </c>
       <c r="I3">
-        <v>1.9</v>
+        <v>1.96</v>
       </c>
       <c r="J3">
-        <v>1.95</v>
+        <v>1.92</v>
+      </c>
+      <c r="K3">
+        <v>2.87</v>
+      </c>
+      <c r="L3">
+        <v>1.79</v>
+      </c>
+      <c r="M3">
+        <v>1.75</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1883,31 +1992,40 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>20.86</v>
+        <v>20.81</v>
       </c>
       <c r="C4">
-        <v>13.93</v>
+        <v>13.87</v>
       </c>
       <c r="D4">
-        <v>13.79</v>
+        <v>13.87</v>
       </c>
       <c r="E4">
-        <v>23.69</v>
+        <v>23.64</v>
       </c>
       <c r="F4">
-        <v>17.46</v>
+        <v>17.63</v>
       </c>
       <c r="G4">
-        <v>17.2</v>
+        <v>17.149999999999999</v>
       </c>
       <c r="H4">
-        <v>27.89</v>
+        <v>27.56</v>
       </c>
       <c r="I4">
-        <v>18.82</v>
+        <v>19</v>
       </c>
       <c r="J4">
-        <v>18.84</v>
+        <v>18.760000000000002</v>
+      </c>
+      <c r="K4">
+        <v>38.51</v>
+      </c>
+      <c r="L4">
+        <v>19.559999999999999</v>
+      </c>
+      <c r="M4">
+        <v>18.989999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1915,7 +2033,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>9.61</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="C5" t="e">
         <v>#N/A</v>
@@ -1924,7 +2042,7 @@
         <v>#N/A</v>
       </c>
       <c r="E5">
-        <v>7.65</v>
+        <v>7.6</v>
       </c>
       <c r="F5" t="e">
         <v>#N/A</v>
@@ -1933,12 +2051,21 @@
         <v>#N/A</v>
       </c>
       <c r="H5">
-        <v>21.35</v>
+        <v>21.29</v>
       </c>
       <c r="I5" t="e">
         <v>#N/A</v>
       </c>
       <c r="J5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K5">
+        <v>10.75</v>
+      </c>
+      <c r="L5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M5" t="e">
         <v>#N/A</v>
       </c>
     </row>
@@ -1964,14 +2091,23 @@
       <c r="G6" t="e">
         <v>#N/A</v>
       </c>
-      <c r="H6">
-        <v>0.99</v>
-      </c>
-      <c r="I6">
-        <v>0.37</v>
-      </c>
-      <c r="J6">
-        <v>0.38</v>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1979,31 +2115,40 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>8.8800000000000008</v>
+        <v>9.1199999999999992</v>
       </c>
       <c r="C7">
-        <v>3.26</v>
+        <v>3.39</v>
       </c>
       <c r="D7">
-        <v>3.12</v>
+        <v>3.68</v>
       </c>
       <c r="E7">
-        <v>14.58</v>
+        <v>13.92</v>
       </c>
       <c r="F7">
-        <v>4.07</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="G7">
-        <v>3.87</v>
+        <v>3.91</v>
       </c>
       <c r="H7">
-        <v>32.090000000000003</v>
+        <v>32.04</v>
       </c>
       <c r="I7">
-        <v>6.26</v>
+        <v>6.28</v>
       </c>
       <c r="J7">
-        <v>6.1</v>
+        <v>5.73</v>
+      </c>
+      <c r="K7">
+        <v>22</v>
+      </c>
+      <c r="L7">
+        <v>5.55</v>
+      </c>
+      <c r="M7">
+        <v>5.23</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2011,31 +2156,40 @@
         <v>19</v>
       </c>
       <c r="B8">
-        <v>3.15</v>
+        <v>3.12</v>
       </c>
       <c r="C8">
         <v>1.24</v>
       </c>
       <c r="D8">
-        <v>1.22</v>
+        <v>1.24</v>
       </c>
       <c r="E8">
-        <v>4.54</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="F8">
+        <v>1.34</v>
+      </c>
+      <c r="G8">
         <v>1.38</v>
       </c>
-      <c r="G8">
-        <v>1.36</v>
-      </c>
       <c r="H8">
-        <v>17.489999999999998</v>
+        <v>18.62</v>
       </c>
       <c r="I8">
         <v>2.76</v>
       </c>
       <c r="J8">
         <v>2.73</v>
+      </c>
+      <c r="K8">
+        <v>6.2</v>
+      </c>
+      <c r="L8">
+        <v>1.38</v>
+      </c>
+      <c r="M8">
+        <v>1.36</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2043,85 +2197,40 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>59.57</v>
+        <v>59.06</v>
       </c>
       <c r="C9">
-        <v>24.69</v>
+        <v>24.63</v>
       </c>
       <c r="D9">
-        <v>22.84</v>
+        <v>22.74</v>
       </c>
       <c r="E9">
-        <v>94.27</v>
+        <v>95.33</v>
       </c>
       <c r="F9">
-        <v>27.76</v>
+        <v>27.59</v>
       </c>
       <c r="G9" t="e">
         <v>#N/A</v>
       </c>
       <c r="H9">
-        <v>338.14</v>
+        <v>340.57</v>
       </c>
       <c r="I9">
-        <v>45.52</v>
+        <v>45.56</v>
       </c>
       <c r="J9">
-        <v>35.93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="D16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="D17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="D18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>28</v>
+        <v>35.840000000000003</v>
+      </c>
+      <c r="K9">
+        <v>145.88</v>
+      </c>
+      <c r="L9">
+        <v>33.380000000000003</v>
+      </c>
+      <c r="M9">
+        <v>81.099999999999994</v>
       </c>
     </row>
   </sheetData>
@@ -2132,12 +2241,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F98251-3BCB-4E2C-93DA-53EFA4B6B58E}">
-  <dimension ref="A1:M9"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E4BC65-974B-4C0A-9F10-9CAD64070E0C}">
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,40 +2311,2362 @@
       <c r="A2" t="s">
         <v>13</v>
       </c>
+      <c r="B2">
+        <v>103.57</v>
+      </c>
+      <c r="C2">
+        <v>56.25</v>
+      </c>
+      <c r="D2">
+        <v>50.7</v>
+      </c>
+      <c r="E2">
+        <v>125.33</v>
+      </c>
+      <c r="F2">
+        <v>51.5</v>
+      </c>
+      <c r="G2">
+        <v>47.56</v>
+      </c>
+      <c r="H2">
+        <v>304.19</v>
+      </c>
+      <c r="I2">
+        <v>107.32</v>
+      </c>
+      <c r="J2">
+        <v>88.19</v>
+      </c>
+      <c r="K2">
+        <v>182.36</v>
+      </c>
+      <c r="L2">
+        <v>65.86</v>
+      </c>
+      <c r="M2">
+        <v>58.35</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
+      <c r="B3">
+        <v>2.29</v>
+      </c>
+      <c r="C3">
+        <v>0.77</v>
+      </c>
+      <c r="D3">
+        <v>0.75</v>
+      </c>
+      <c r="E3">
+        <v>2.14</v>
+      </c>
+      <c r="F3">
+        <v>0.96</v>
+      </c>
+      <c r="G3">
+        <v>0.96</v>
+      </c>
+      <c r="H3">
+        <v>5.4</v>
+      </c>
+      <c r="I3">
+        <v>1.9</v>
+      </c>
+      <c r="J3">
+        <v>1.95</v>
+      </c>
+      <c r="K3">
+        <v>2.86</v>
+      </c>
+      <c r="L3">
+        <v>1.76</v>
+      </c>
+      <c r="M3">
+        <v>1.77</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
+      <c r="B4">
+        <v>20.86</v>
+      </c>
+      <c r="C4">
+        <v>13.93</v>
+      </c>
+      <c r="D4">
+        <v>13.79</v>
+      </c>
+      <c r="E4">
+        <v>23.69</v>
+      </c>
+      <c r="F4">
+        <v>17.46</v>
+      </c>
+      <c r="G4">
+        <v>17.2</v>
+      </c>
+      <c r="H4">
+        <v>27.89</v>
+      </c>
+      <c r="I4">
+        <v>18.82</v>
+      </c>
+      <c r="J4">
+        <v>18.84</v>
+      </c>
+      <c r="K4">
+        <v>38.31</v>
+      </c>
+      <c r="L4">
+        <v>19.63</v>
+      </c>
+      <c r="M4">
+        <v>18.93</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
+      <c r="B5">
+        <v>9.61</v>
+      </c>
+      <c r="C5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E5">
+        <v>7.65</v>
+      </c>
+      <c r="F5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H5">
+        <v>21.35</v>
+      </c>
+      <c r="I5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K5">
+        <v>11.11</v>
+      </c>
+      <c r="L5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M5" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
+      <c r="B6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
+      <c r="B7">
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="C7">
+        <v>3.26</v>
+      </c>
+      <c r="D7">
+        <v>3.12</v>
+      </c>
+      <c r="E7">
+        <v>14.58</v>
+      </c>
+      <c r="F7">
+        <v>4.07</v>
+      </c>
+      <c r="G7">
+        <v>3.87</v>
+      </c>
+      <c r="H7">
+        <v>32.090000000000003</v>
+      </c>
+      <c r="I7">
+        <v>6.26</v>
+      </c>
+      <c r="J7">
+        <v>6.1</v>
+      </c>
+      <c r="K7">
+        <v>21.91</v>
+      </c>
+      <c r="L7">
+        <v>5.54</v>
+      </c>
+      <c r="M7">
+        <v>5.2</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
+      <c r="B8">
+        <v>3.15</v>
+      </c>
+      <c r="C8">
+        <v>1.24</v>
+      </c>
+      <c r="D8">
+        <v>1.22</v>
+      </c>
+      <c r="E8">
+        <v>4.54</v>
+      </c>
+      <c r="F8">
+        <v>1.38</v>
+      </c>
+      <c r="G8">
+        <v>1.36</v>
+      </c>
+      <c r="H8">
+        <v>17.489999999999998</v>
+      </c>
+      <c r="I8">
+        <v>2.76</v>
+      </c>
+      <c r="J8">
+        <v>2.73</v>
+      </c>
+      <c r="K8">
+        <v>6.23</v>
+      </c>
+      <c r="L8">
+        <v>1.36</v>
+      </c>
+      <c r="M8">
+        <v>1.33</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
+      </c>
+      <c r="B9">
+        <v>59.57</v>
+      </c>
+      <c r="C9">
+        <v>24.69</v>
+      </c>
+      <c r="D9">
+        <v>22.84</v>
+      </c>
+      <c r="E9">
+        <v>94.27</v>
+      </c>
+      <c r="F9">
+        <v>27.76</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H9">
+        <v>338.14</v>
+      </c>
+      <c r="I9">
+        <v>45.52</v>
+      </c>
+      <c r="J9">
+        <v>35.93</v>
+      </c>
+      <c r="K9">
+        <v>147.37</v>
+      </c>
+      <c r="L9">
+        <v>33.5</v>
+      </c>
+      <c r="M9">
+        <v>80.709999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F98251-3BCB-4E2C-93DA-53EFA4B6B58E}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>102.3</v>
+      </c>
+      <c r="C2">
+        <v>56.21</v>
+      </c>
+      <c r="D2">
+        <v>50.08</v>
+      </c>
+      <c r="E2">
+        <v>124.28</v>
+      </c>
+      <c r="F2">
+        <v>52.61</v>
+      </c>
+      <c r="G2">
+        <v>47.83</v>
+      </c>
+      <c r="H2">
+        <v>306.45</v>
+      </c>
+      <c r="I2">
+        <v>108.43</v>
+      </c>
+      <c r="J2">
+        <v>89.8</v>
+      </c>
+      <c r="K2">
+        <v>183.55</v>
+      </c>
+      <c r="L2">
+        <v>66.55</v>
+      </c>
+      <c r="M2">
+        <v>57.83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="C3">
+        <v>0.75</v>
+      </c>
+      <c r="D3">
+        <v>0.75</v>
+      </c>
+      <c r="E3">
+        <v>2.1</v>
+      </c>
+      <c r="F3">
+        <v>0.97</v>
+      </c>
+      <c r="G3">
+        <v>0.99</v>
+      </c>
+      <c r="H3">
+        <v>5.5</v>
+      </c>
+      <c r="I3">
+        <v>1.94</v>
+      </c>
+      <c r="J3">
+        <v>1.99</v>
+      </c>
+      <c r="K3">
+        <v>3.18</v>
+      </c>
+      <c r="L3">
+        <v>1.75</v>
+      </c>
+      <c r="M3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>20.86</v>
+      </c>
+      <c r="C4">
+        <v>13.84</v>
+      </c>
+      <c r="D4">
+        <v>13.65</v>
+      </c>
+      <c r="E4">
+        <v>23.82</v>
+      </c>
+      <c r="F4">
+        <v>17.510000000000002</v>
+      </c>
+      <c r="G4">
+        <v>17.28</v>
+      </c>
+      <c r="H4">
+        <v>28.19</v>
+      </c>
+      <c r="I4">
+        <v>18.87</v>
+      </c>
+      <c r="J4">
+        <v>19.03</v>
+      </c>
+      <c r="K4">
+        <v>38.36</v>
+      </c>
+      <c r="L4">
+        <v>19.7</v>
+      </c>
+      <c r="M4">
+        <v>19.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>9.73</v>
+      </c>
+      <c r="C5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E5">
+        <v>7.62</v>
+      </c>
+      <c r="F5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H5">
+        <v>21.88</v>
+      </c>
+      <c r="I5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K5">
+        <v>10.79</v>
+      </c>
+      <c r="L5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="C7">
+        <v>3.37</v>
+      </c>
+      <c r="D7">
+        <v>3.12</v>
+      </c>
+      <c r="E7">
+        <v>14.04</v>
+      </c>
+      <c r="F7">
+        <v>4.05</v>
+      </c>
+      <c r="G7">
+        <v>3.9</v>
+      </c>
+      <c r="H7">
+        <v>32.049999999999997</v>
+      </c>
+      <c r="I7">
+        <v>6.24</v>
+      </c>
+      <c r="J7">
+        <v>5.76</v>
+      </c>
+      <c r="K7">
+        <v>22.29</v>
+      </c>
+      <c r="L7">
+        <v>5.57</v>
+      </c>
+      <c r="M7">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>3.13</v>
+      </c>
+      <c r="C8">
+        <v>1.25</v>
+      </c>
+      <c r="D8">
+        <v>1.22</v>
+      </c>
+      <c r="E8">
+        <v>4.24</v>
+      </c>
+      <c r="F8">
+        <v>1.33</v>
+      </c>
+      <c r="G8">
+        <v>1.36</v>
+      </c>
+      <c r="H8">
+        <v>17.61</v>
+      </c>
+      <c r="I8">
+        <v>2.77</v>
+      </c>
+      <c r="J8">
+        <v>2.76</v>
+      </c>
+      <c r="K8">
+        <v>6.23</v>
+      </c>
+      <c r="L8">
+        <v>1.34</v>
+      </c>
+      <c r="M8">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>59.22</v>
+      </c>
+      <c r="C9">
+        <v>24.73</v>
+      </c>
+      <c r="D9">
+        <v>22.8</v>
+      </c>
+      <c r="E9">
+        <v>94.36</v>
+      </c>
+      <c r="F9">
+        <v>27.93</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H9">
+        <v>338.38</v>
+      </c>
+      <c r="I9">
+        <v>45.31</v>
+      </c>
+      <c r="J9">
+        <v>36.08</v>
+      </c>
+      <c r="K9">
+        <v>146.55000000000001</v>
+      </c>
+      <c r="L9">
+        <v>34.450000000000003</v>
+      </c>
+      <c r="M9">
+        <v>80.959999999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67910417-35FF-498D-853B-7A218C528C4D}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>102.8</v>
+      </c>
+      <c r="C2">
+        <v>57.76</v>
+      </c>
+      <c r="D2">
+        <v>50.6</v>
+      </c>
+      <c r="E2">
+        <v>124.59</v>
+      </c>
+      <c r="F2">
+        <v>52.13</v>
+      </c>
+      <c r="G2">
+        <v>47.49</v>
+      </c>
+      <c r="H2">
+        <v>303.45999999999998</v>
+      </c>
+      <c r="I2">
+        <v>107.43</v>
+      </c>
+      <c r="J2">
+        <v>88.37</v>
+      </c>
+      <c r="K2">
+        <v>181.24</v>
+      </c>
+      <c r="L2">
+        <v>66.84</v>
+      </c>
+      <c r="M2">
+        <v>58.07</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>2.17</v>
+      </c>
+      <c r="C3">
+        <v>0.76</v>
+      </c>
+      <c r="D3">
+        <v>0.76</v>
+      </c>
+      <c r="E3">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="F3">
+        <v>0.96</v>
+      </c>
+      <c r="G3">
+        <v>0.93</v>
+      </c>
+      <c r="H3">
+        <v>5.51</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>1.9</v>
+      </c>
+      <c r="K3">
+        <v>2.91</v>
+      </c>
+      <c r="L3">
+        <v>1.76</v>
+      </c>
+      <c r="M3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>21.17</v>
+      </c>
+      <c r="C4">
+        <v>13.87</v>
+      </c>
+      <c r="D4">
+        <v>13.68</v>
+      </c>
+      <c r="E4">
+        <v>23.76</v>
+      </c>
+      <c r="F4">
+        <v>17.54</v>
+      </c>
+      <c r="G4">
+        <v>17.2</v>
+      </c>
+      <c r="H4">
+        <v>27.63</v>
+      </c>
+      <c r="I4">
+        <v>18.96</v>
+      </c>
+      <c r="J4">
+        <v>18.78</v>
+      </c>
+      <c r="K4">
+        <v>38.39</v>
+      </c>
+      <c r="L4">
+        <v>19.71</v>
+      </c>
+      <c r="M4">
+        <v>19.079999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>9.75</v>
+      </c>
+      <c r="C5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E5">
+        <v>7.59</v>
+      </c>
+      <c r="F5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H5">
+        <v>21.71</v>
+      </c>
+      <c r="I5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K5">
+        <v>11.07</v>
+      </c>
+      <c r="L5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>8.91</v>
+      </c>
+      <c r="C7">
+        <v>3.3</v>
+      </c>
+      <c r="D7">
+        <v>3.13</v>
+      </c>
+      <c r="E7">
+        <v>14.14</v>
+      </c>
+      <c r="F7">
+        <v>4.07</v>
+      </c>
+      <c r="G7">
+        <v>3.87</v>
+      </c>
+      <c r="H7">
+        <v>32.28</v>
+      </c>
+      <c r="I7">
+        <v>6.23</v>
+      </c>
+      <c r="J7">
+        <v>5.75</v>
+      </c>
+      <c r="K7">
+        <v>22.1</v>
+      </c>
+      <c r="L7">
+        <v>5.57</v>
+      </c>
+      <c r="M7">
+        <v>5.28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>3.24</v>
+      </c>
+      <c r="C8">
+        <v>1.24</v>
+      </c>
+      <c r="D8">
+        <v>1.24</v>
+      </c>
+      <c r="E8">
+        <v>4.28</v>
+      </c>
+      <c r="F8">
+        <v>1.32</v>
+      </c>
+      <c r="G8">
+        <v>1.39</v>
+      </c>
+      <c r="H8">
+        <v>17.62</v>
+      </c>
+      <c r="I8">
+        <v>2.73</v>
+      </c>
+      <c r="J8">
+        <v>2.73</v>
+      </c>
+      <c r="K8">
+        <v>6.25</v>
+      </c>
+      <c r="L8">
+        <v>1.37</v>
+      </c>
+      <c r="M8">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>59.49</v>
+      </c>
+      <c r="C9">
+        <v>24.56</v>
+      </c>
+      <c r="D9">
+        <v>23.51</v>
+      </c>
+      <c r="E9">
+        <v>95.1</v>
+      </c>
+      <c r="F9">
+        <v>28.14</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H9">
+        <v>337.34</v>
+      </c>
+      <c r="I9">
+        <v>45.27</v>
+      </c>
+      <c r="J9">
+        <v>36.21</v>
+      </c>
+      <c r="K9">
+        <v>144</v>
+      </c>
+      <c r="L9">
+        <v>33.81</v>
+      </c>
+      <c r="M9">
+        <v>81.14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B2153B5-2C46-4DED-8DFE-DF284EA32F4A}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>102.68</v>
+      </c>
+      <c r="C2">
+        <v>57.44</v>
+      </c>
+      <c r="D2">
+        <v>50.01</v>
+      </c>
+      <c r="E2">
+        <v>124.63</v>
+      </c>
+      <c r="F2">
+        <v>52.02</v>
+      </c>
+      <c r="G2">
+        <v>47.65</v>
+      </c>
+      <c r="H2">
+        <v>304.97000000000003</v>
+      </c>
+      <c r="I2">
+        <v>107.76</v>
+      </c>
+      <c r="J2">
+        <v>88.59</v>
+      </c>
+      <c r="K2">
+        <v>184.52</v>
+      </c>
+      <c r="L2">
+        <v>66.459999999999994</v>
+      </c>
+      <c r="M2">
+        <v>57.97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>2.21</v>
+      </c>
+      <c r="C3">
+        <v>0.77</v>
+      </c>
+      <c r="D3">
+        <v>0.77</v>
+      </c>
+      <c r="E3">
+        <v>2.16</v>
+      </c>
+      <c r="F3">
+        <v>0.97</v>
+      </c>
+      <c r="G3">
+        <v>0.9</v>
+      </c>
+      <c r="H3">
+        <v>5.51</v>
+      </c>
+      <c r="I3">
+        <v>2.09</v>
+      </c>
+      <c r="J3">
+        <v>1.91</v>
+      </c>
+      <c r="K3">
+        <v>2.86</v>
+      </c>
+      <c r="L3">
+        <v>1.77</v>
+      </c>
+      <c r="M3">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>20.87</v>
+      </c>
+      <c r="C4">
+        <v>13.89</v>
+      </c>
+      <c r="D4">
+        <v>13.81</v>
+      </c>
+      <c r="E4">
+        <v>23.7</v>
+      </c>
+      <c r="F4">
+        <v>17.48</v>
+      </c>
+      <c r="G4">
+        <v>17.260000000000002</v>
+      </c>
+      <c r="H4">
+        <v>27.9</v>
+      </c>
+      <c r="I4">
+        <v>18.87</v>
+      </c>
+      <c r="J4">
+        <v>18.75</v>
+      </c>
+      <c r="K4">
+        <v>38.29</v>
+      </c>
+      <c r="L4">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="M4">
+        <v>19.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>9.69</v>
+      </c>
+      <c r="C5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E5">
+        <v>7.66</v>
+      </c>
+      <c r="F5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H5">
+        <v>21.32</v>
+      </c>
+      <c r="I5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K5">
+        <v>10.73</v>
+      </c>
+      <c r="L5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>8.89</v>
+      </c>
+      <c r="C7">
+        <v>3.32</v>
+      </c>
+      <c r="D7">
+        <v>3.11</v>
+      </c>
+      <c r="E7">
+        <v>14.11</v>
+      </c>
+      <c r="F7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G7">
+        <v>3.88</v>
+      </c>
+      <c r="H7">
+        <v>32.04</v>
+      </c>
+      <c r="I7">
+        <v>6.32</v>
+      </c>
+      <c r="J7">
+        <v>5.79</v>
+      </c>
+      <c r="K7">
+        <v>21.87</v>
+      </c>
+      <c r="L7">
+        <v>5.53</v>
+      </c>
+      <c r="M7">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>3.12</v>
+      </c>
+      <c r="C8">
+        <v>1.24</v>
+      </c>
+      <c r="D8">
+        <v>1.22</v>
+      </c>
+      <c r="E8">
+        <v>4.25</v>
+      </c>
+      <c r="F8">
+        <v>1.35</v>
+      </c>
+      <c r="G8">
+        <v>1.38</v>
+      </c>
+      <c r="H8">
+        <v>17.86</v>
+      </c>
+      <c r="I8">
+        <v>2.77</v>
+      </c>
+      <c r="J8">
+        <v>2.75</v>
+      </c>
+      <c r="K8">
+        <v>6.22</v>
+      </c>
+      <c r="L8">
+        <v>1.35</v>
+      </c>
+      <c r="M8">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>59.34</v>
+      </c>
+      <c r="C9">
+        <v>24.62</v>
+      </c>
+      <c r="D9">
+        <v>24.11</v>
+      </c>
+      <c r="E9">
+        <v>94.12</v>
+      </c>
+      <c r="F9">
+        <v>27.74</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H9">
+        <v>340.51</v>
+      </c>
+      <c r="I9">
+        <v>46.37</v>
+      </c>
+      <c r="J9">
+        <v>35.950000000000003</v>
+      </c>
+      <c r="K9">
+        <v>143.53</v>
+      </c>
+      <c r="L9">
+        <v>33.35</v>
+      </c>
+      <c r="M9">
+        <v>80.930000000000007</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7FF9B2-F565-4791-A51B-4BA1CCAD0D60}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>102.55</v>
+      </c>
+      <c r="C2">
+        <v>56.36</v>
+      </c>
+      <c r="D2">
+        <v>50.87</v>
+      </c>
+      <c r="E2">
+        <v>123.93</v>
+      </c>
+      <c r="F2">
+        <v>52.15</v>
+      </c>
+      <c r="G2">
+        <v>47.42</v>
+      </c>
+      <c r="H2">
+        <v>303.43</v>
+      </c>
+      <c r="I2">
+        <v>107.46</v>
+      </c>
+      <c r="J2">
+        <v>88.96</v>
+      </c>
+      <c r="K2">
+        <v>183.75</v>
+      </c>
+      <c r="L2">
+        <v>66.91</v>
+      </c>
+      <c r="M2">
+        <v>57.65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>2.14</v>
+      </c>
+      <c r="C3">
+        <v>0.76</v>
+      </c>
+      <c r="D3">
+        <v>0.76</v>
+      </c>
+      <c r="E3">
+        <v>2.09</v>
+      </c>
+      <c r="F3">
+        <v>0.95</v>
+      </c>
+      <c r="G3">
+        <v>0.92</v>
+      </c>
+      <c r="H3">
+        <v>5.38</v>
+      </c>
+      <c r="I3">
+        <v>1.96</v>
+      </c>
+      <c r="J3">
+        <v>1.98</v>
+      </c>
+      <c r="K3">
+        <v>3.25</v>
+      </c>
+      <c r="L3">
+        <v>1.75</v>
+      </c>
+      <c r="M3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>20.76</v>
+      </c>
+      <c r="C4">
+        <v>13.85</v>
+      </c>
+      <c r="D4">
+        <v>13.75</v>
+      </c>
+      <c r="E4">
+        <v>23.72</v>
+      </c>
+      <c r="F4">
+        <v>17.489999999999998</v>
+      </c>
+      <c r="G4">
+        <v>17.37</v>
+      </c>
+      <c r="H4">
+        <v>27.56</v>
+      </c>
+      <c r="I4">
+        <v>19.04</v>
+      </c>
+      <c r="J4">
+        <v>18.86</v>
+      </c>
+      <c r="K4">
+        <v>38.450000000000003</v>
+      </c>
+      <c r="L4">
+        <v>19.63</v>
+      </c>
+      <c r="M4">
+        <v>18.97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E5">
+        <v>7.72</v>
+      </c>
+      <c r="F5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H5">
+        <v>21.3</v>
+      </c>
+      <c r="I5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K5">
+        <v>11</v>
+      </c>
+      <c r="L5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>8.86</v>
+      </c>
+      <c r="C7">
+        <v>3.29</v>
+      </c>
+      <c r="D7">
+        <v>3.11</v>
+      </c>
+      <c r="E7">
+        <v>13.9</v>
+      </c>
+      <c r="F7">
+        <v>4.08</v>
+      </c>
+      <c r="G7">
+        <v>3.97</v>
+      </c>
+      <c r="H7">
+        <v>32.07</v>
+      </c>
+      <c r="I7">
+        <v>6.28</v>
+      </c>
+      <c r="J7">
+        <v>5.74</v>
+      </c>
+      <c r="K7">
+        <v>21.95</v>
+      </c>
+      <c r="L7">
+        <v>5.53</v>
+      </c>
+      <c r="M7">
+        <v>5.23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>3.17</v>
+      </c>
+      <c r="C8">
+        <v>1.24</v>
+      </c>
+      <c r="D8">
+        <v>1.22</v>
+      </c>
+      <c r="E8">
+        <v>4.34</v>
+      </c>
+      <c r="F8">
+        <v>1.32</v>
+      </c>
+      <c r="G8">
+        <v>1.36</v>
+      </c>
+      <c r="H8">
+        <v>17.78</v>
+      </c>
+      <c r="I8">
+        <v>2.73</v>
+      </c>
+      <c r="J8">
+        <v>2.7</v>
+      </c>
+      <c r="K8">
+        <v>6.21</v>
+      </c>
+      <c r="L8">
+        <v>1.34</v>
+      </c>
+      <c r="M8">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>59.26</v>
+      </c>
+      <c r="C9">
+        <v>26.02</v>
+      </c>
+      <c r="D9">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <v>95.75</v>
+      </c>
+      <c r="F9">
+        <v>27.7</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H9">
+        <v>338.64</v>
+      </c>
+      <c r="I9">
+        <v>48.55</v>
+      </c>
+      <c r="J9">
+        <v>36.08</v>
+      </c>
+      <c r="K9">
+        <v>148.09</v>
+      </c>
+      <c r="L9">
+        <v>33.479999999999997</v>
+      </c>
+      <c r="M9">
+        <v>80.89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DBF310-6C1C-404F-8B67-EB9DDCC1058F}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>104.26</v>
+      </c>
+      <c r="C2">
+        <v>56.99</v>
+      </c>
+      <c r="D2">
+        <v>50.08</v>
+      </c>
+      <c r="E2">
+        <v>123.95</v>
+      </c>
+      <c r="F2">
+        <v>52.03</v>
+      </c>
+      <c r="G2">
+        <v>47.44</v>
+      </c>
+      <c r="H2">
+        <v>308.60000000000002</v>
+      </c>
+      <c r="I2">
+        <v>109.29</v>
+      </c>
+      <c r="J2">
+        <v>89.65</v>
+      </c>
+      <c r="K2">
+        <v>181.04</v>
+      </c>
+      <c r="L2">
+        <v>66.02</v>
+      </c>
+      <c r="M2">
+        <v>58.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>2.23</v>
+      </c>
+      <c r="C3">
+        <v>0.76</v>
+      </c>
+      <c r="D3">
+        <v>0.77</v>
+      </c>
+      <c r="E3">
+        <v>2.21</v>
+      </c>
+      <c r="F3">
+        <v>0.98</v>
+      </c>
+      <c r="G3">
+        <v>0.91</v>
+      </c>
+      <c r="H3">
+        <v>5.55</v>
+      </c>
+      <c r="I3">
+        <v>1.9</v>
+      </c>
+      <c r="J3">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="K3">
+        <v>2.89</v>
+      </c>
+      <c r="L3">
+        <v>1.75</v>
+      </c>
+      <c r="M3">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>20.82</v>
+      </c>
+      <c r="C4">
+        <v>13.9</v>
+      </c>
+      <c r="D4">
+        <v>13.94</v>
+      </c>
+      <c r="E4">
+        <v>23.67</v>
+      </c>
+      <c r="F4">
+        <v>17.71</v>
+      </c>
+      <c r="G4">
+        <v>17.29</v>
+      </c>
+      <c r="H4">
+        <v>27.62</v>
+      </c>
+      <c r="I4">
+        <v>19.149999999999999</v>
+      </c>
+      <c r="J4">
+        <v>18.75</v>
+      </c>
+      <c r="K4">
+        <v>38.57</v>
+      </c>
+      <c r="L4">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="M4">
+        <v>19.010000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>9.77</v>
+      </c>
+      <c r="C5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E5">
+        <v>7.61</v>
+      </c>
+      <c r="F5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H5">
+        <v>21.62</v>
+      </c>
+      <c r="I5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K5">
+        <v>10.74</v>
+      </c>
+      <c r="L5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="F6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>9.16</v>
+      </c>
+      <c r="C7">
+        <v>3.27</v>
+      </c>
+      <c r="D7">
+        <v>3.12</v>
+      </c>
+      <c r="E7">
+        <v>13.82</v>
+      </c>
+      <c r="F7">
+        <v>4.49</v>
+      </c>
+      <c r="G7">
+        <v>3.95</v>
+      </c>
+      <c r="H7">
+        <v>31.89</v>
+      </c>
+      <c r="I7">
+        <v>6.24</v>
+      </c>
+      <c r="J7">
+        <v>5.76</v>
+      </c>
+      <c r="K7">
+        <v>22.85</v>
+      </c>
+      <c r="L7">
+        <v>5.52</v>
+      </c>
+      <c r="M7">
+        <v>5.24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>3.12</v>
+      </c>
+      <c r="C8">
+        <v>1.24</v>
+      </c>
+      <c r="D8">
+        <v>1.22</v>
+      </c>
+      <c r="E8">
+        <v>4.26</v>
+      </c>
+      <c r="F8">
+        <v>1.36</v>
+      </c>
+      <c r="G8">
+        <v>1.38</v>
+      </c>
+      <c r="H8">
+        <v>17.72</v>
+      </c>
+      <c r="I8">
+        <v>2.74</v>
+      </c>
+      <c r="J8">
+        <v>2.72</v>
+      </c>
+      <c r="K8">
+        <v>7.39</v>
+      </c>
+      <c r="L8">
+        <v>1.34</v>
+      </c>
+      <c r="M8">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>59.45</v>
+      </c>
+      <c r="C9">
+        <v>24.58</v>
+      </c>
+      <c r="D9">
+        <v>22.7</v>
+      </c>
+      <c r="E9">
+        <v>94.82</v>
+      </c>
+      <c r="F9">
+        <v>27.8</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H9">
+        <v>338.21</v>
+      </c>
+      <c r="I9">
+        <v>45.47</v>
+      </c>
+      <c r="J9">
+        <v>36.19</v>
+      </c>
+      <c r="K9">
+        <v>145.83000000000001</v>
+      </c>
+      <c r="L9">
+        <v>33.57</v>
+      </c>
+      <c r="M9">
+        <v>82.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>